<commit_message>
added earliest filing date temporily
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -140,10 +140,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>186.0</v>
+        <v>187.0</v>
       </c>
       <c r="F2" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
     </row>
     <row r="3">
@@ -160,10 +160,10 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>113.0</v>
+        <v>112.0</v>
       </c>
       <c r="F3" t="n">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fixes in wipo api reader
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>RAP - Company ID</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Total number of Citations</t>
   </si>
   <si>
-    <t>1</t>
+    <t>1, 2</t>
   </si>
   <si>
     <t>阿尔特汽车技术股份有限公司；阿尔特(中国)汽车技术有限公司</t>
@@ -41,13 +41,118 @@
     <t>IAT (China) Automobile Technology Co. Ltd.</t>
   </si>
   <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>中国银行股份有限公司</t>
-  </si>
-  <si>
-    <t>Bank of China Limited</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>19团</t>
+  </si>
+  <si>
+    <t>19 Tuan.com</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>十九楼网络股份有限公司；杭州十九楼网络传媒有限公司</t>
+  </si>
+  <si>
+    <t>19lou Network Media Co., Ltd;Hangzhou 19lou Network Media Co., Ltd.</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>贰壹叁壹伍（北京）征信管理集团股份有限公司</t>
+  </si>
+  <si>
+    <t>21315 Credit Management Co., Ltd.</t>
+  </si>
+  <si>
+    <t>6, 7, 8, 9</t>
+  </si>
+  <si>
+    <t>北京世纪互联宽带数据中心；北京世纪互联工程技术服务有限公司</t>
+  </si>
+  <si>
+    <t>21ViaNet</t>
+  </si>
+  <si>
+    <t>10, 11</t>
+  </si>
+  <si>
+    <t>360圈</t>
+  </si>
+  <si>
+    <t>360quan.com</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>360圈网</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>上海震撼广告传播有限公司</t>
+  </si>
+  <si>
+    <t>3D Media (China) Ltd.</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>商埃曲网络软件(上海)有限公司</t>
+  </si>
+  <si>
+    <t>3H International Technology (Shanghai) Co., Ltd.</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>递四方速递有限公司</t>
+  </si>
+  <si>
+    <t>4PX EXPRESS Co., Ltd.</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5151团购网  </t>
+  </si>
+  <si>
+    <t>5151tuan.com</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>广州市千钧网络科技有限公司</t>
+  </si>
+  <si>
+    <t>56.com Inc.</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>数银在线有限公司  </t>
+  </si>
+  <si>
+    <t>6677Bank Online Co., Ltd.</t>
+  </si>
+  <si>
+    <t>19, 20, 21, 22</t>
+  </si>
+  <si>
+    <t>7天连锁酒店集团；七天酒店（深圳）有限公司 </t>
+  </si>
+  <si>
+    <t>7 Days Group Holdings Limited</t>
   </si>
 </sst>
 </file>
@@ -100,8 +205,8 @@
   <cols>
     <col min="1" max="1" width="17.16796875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.37109375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="61.76953125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="39.83203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="64.8359375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="65.109375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="22.75" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="23.86328125" customWidth="true" bestFit="true"/>
   </cols>
@@ -160,10 +265,250 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>112.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all rest features
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -31349,10 +31349,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>153.0</v>
+        <v>152.0</v>
       </c>
       <c r="F2" t="n">
-        <v>58.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="3">
@@ -31509,10 +31509,10 @@
         <v>31</v>
       </c>
       <c r="E10" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -31729,10 +31729,10 @@
         <v>64</v>
       </c>
       <c r="E21" t="n">
-        <v>27.0</v>
+        <v>0.0</v>
       </c>
       <c r="F21" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="22">
@@ -31769,10 +31769,10 @@
         <v>70</v>
       </c>
       <c r="E23" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F23" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="24">
@@ -31809,10 +31809,10 @@
         <v>76</v>
       </c>
       <c r="E25" t="n">
-        <v>135.0</v>
+        <v>0.0</v>
       </c>
       <c r="F25" t="n">
-        <v>72.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
@@ -31849,10 +31849,10 @@
         <v>82</v>
       </c>
       <c r="E27" t="n">
-        <v>308.0</v>
+        <v>0.0</v>
       </c>
       <c r="F27" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
@@ -31869,10 +31869,10 @@
         <v>85</v>
       </c>
       <c r="E28" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="F28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="29">
@@ -31889,10 +31889,10 @@
         <v>88</v>
       </c>
       <c r="E29" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="F29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
@@ -64449,10 +64449,10 @@
         <v>4948</v>
       </c>
       <c r="E1657" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1657" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1658">
@@ -64469,10 +64469,10 @@
         <v>4951</v>
       </c>
       <c r="E1658" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1658" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1659">
@@ -64489,10 +64489,10 @@
         <v>4954</v>
       </c>
       <c r="E1659" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1659" t="n">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1660">
@@ -64529,10 +64529,10 @@
         <v>4960</v>
       </c>
       <c r="E1661" t="n">
-        <v>91.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1661" t="n">
-        <v>59.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1662">
@@ -64569,7 +64569,7 @@
         <v>4966</v>
       </c>
       <c r="E1663" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1663" t="n">
         <v>0.0</v>
@@ -64589,7 +64589,7 @@
         <v>4969</v>
       </c>
       <c r="E1664" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1664" t="n">
         <v>0.0</v>
@@ -64689,10 +64689,10 @@
         <v>4983</v>
       </c>
       <c r="E1669" t="n">
-        <v>716.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1669" t="n">
-        <v>120.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1670">
@@ -64789,10 +64789,10 @@
         <v>4998</v>
       </c>
       <c r="E1674" t="n">
-        <v>94.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1674" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1675">
@@ -64829,10 +64829,10 @@
         <v>5004</v>
       </c>
       <c r="E1676" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1676" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1677">
@@ -64889,10 +64889,10 @@
         <v>5013</v>
       </c>
       <c r="E1679" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1679" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1680">
@@ -64909,10 +64909,10 @@
         <v>5016</v>
       </c>
       <c r="E1680" t="n">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1680" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1681">
@@ -64949,10 +64949,10 @@
         <v>5022</v>
       </c>
       <c r="E1682" t="n">
-        <v>84.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1682" t="n">
-        <v>58.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1683">
@@ -65089,10 +65089,10 @@
         <v>5043</v>
       </c>
       <c r="E1689" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1689" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1690">
@@ -65149,10 +65149,10 @@
         <v>5052</v>
       </c>
       <c r="E1692" t="n">
-        <v>57.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1692" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1693">
@@ -65229,10 +65229,10 @@
         <v>5064</v>
       </c>
       <c r="E1696" t="n">
-        <v>113.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1696" t="n">
-        <v>425.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1697">
@@ -65269,10 +65269,10 @@
         <v>5070</v>
       </c>
       <c r="E1698" t="n">
-        <v>19.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1698" t="n">
-        <v>29.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1699">
@@ -65369,10 +65369,10 @@
         <v>5085</v>
       </c>
       <c r="E1703" t="n">
-        <v>217.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1703" t="n">
-        <v>208.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1704">
@@ -65429,10 +65429,10 @@
         <v>5094</v>
       </c>
       <c r="E1706" t="n">
-        <v>475.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1706" t="n">
-        <v>118.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1707">
@@ -65449,10 +65449,10 @@
         <v>5097</v>
       </c>
       <c r="E1707" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1707" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1708">
@@ -65509,10 +65509,10 @@
         <v>5106</v>
       </c>
       <c r="E1710" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1710" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1711">
@@ -65609,10 +65609,10 @@
         <v>5121</v>
       </c>
       <c r="E1715" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1715" t="n">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1716">
@@ -65629,7 +65629,7 @@
         <v>5124</v>
       </c>
       <c r="E1716" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1716" t="n">
         <v>0.0</v>
@@ -65649,10 +65649,10 @@
         <v>5127</v>
       </c>
       <c r="E1717" t="n">
-        <v>66.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1717" t="n">
-        <v>25.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1718">
@@ -65689,10 +65689,10 @@
         <v>5133</v>
       </c>
       <c r="E1719" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1719" t="n">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1720">
@@ -65749,7 +65749,7 @@
         <v>5142</v>
       </c>
       <c r="E1722" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1722" t="n">
         <v>0.0</v>
@@ -65769,10 +65769,10 @@
         <v>5145</v>
       </c>
       <c r="E1723" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1723" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1724">
@@ -65789,10 +65789,10 @@
         <v>5148</v>
       </c>
       <c r="E1724" t="n">
-        <v>2627.0</v>
+        <v>0.0</v>
       </c>
       <c r="F1724" t="n">
-        <v>1231.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="1725">
@@ -91529,10 +91529,10 @@
         <v>8989</v>
       </c>
       <c r="E3011" t="n">
-        <v>173.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3011" t="n">
-        <v>145.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3012">
@@ -91549,10 +91549,10 @@
         <v>8992</v>
       </c>
       <c r="E3012" t="n">
-        <v>22.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3012" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3013">
@@ -91609,10 +91609,10 @@
         <v>9001</v>
       </c>
       <c r="E3015" t="n">
-        <v>55.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3015" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3016">
@@ -91689,10 +91689,10 @@
         <v>9013</v>
       </c>
       <c r="E3019" t="n">
-        <v>55.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3019" t="n">
-        <v>38.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3020">
@@ -91749,10 +91749,10 @@
         <v>9022</v>
       </c>
       <c r="E3022" t="n">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3022" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3023">
@@ -91769,10 +91769,10 @@
         <v>9025</v>
       </c>
       <c r="E3023" t="n">
-        <v>17.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3023" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3024">
@@ -91829,10 +91829,10 @@
         <v>9034</v>
       </c>
       <c r="E3026" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3026" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3027">
@@ -91849,10 +91849,10 @@
         <v>9037</v>
       </c>
       <c r="E3027" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3027" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3028">
@@ -91869,10 +91869,10 @@
         <v>9040</v>
       </c>
       <c r="E3028" t="n">
-        <v>82.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3028" t="n">
-        <v>78.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3029">
@@ -100269,10 +100269,10 @@
         <v>10285</v>
       </c>
       <c r="E3448" t="n">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3448" t="n">
-        <v>34.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3449">
@@ -100289,10 +100289,10 @@
         <v>10288</v>
       </c>
       <c r="E3449" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3449" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3450">
@@ -100329,10 +100329,10 @@
         <v>10294</v>
       </c>
       <c r="E3451" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3451" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3452">
@@ -100369,10 +100369,10 @@
         <v>10300</v>
       </c>
       <c r="E3453" t="n">
-        <v>1042.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3453" t="n">
-        <v>515.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3454">
@@ -100409,10 +100409,10 @@
         <v>10306</v>
       </c>
       <c r="E3455" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3455" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3456">
@@ -100529,10 +100529,10 @@
         <v>10323</v>
       </c>
       <c r="E3461" t="n">
-        <v>46.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3461" t="n">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3462">
@@ -100549,10 +100549,10 @@
         <v>10326</v>
       </c>
       <c r="E3462" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3462" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3463">
@@ -100589,10 +100589,10 @@
         <v>10332</v>
       </c>
       <c r="E3464" t="n">
-        <v>162.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3464" t="n">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3465">
@@ -100629,10 +100629,10 @@
         <v>10338</v>
       </c>
       <c r="E3466" t="n">
-        <v>197.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3466" t="n">
-        <v>93.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3467">
@@ -100649,10 +100649,10 @@
         <v>10341</v>
       </c>
       <c r="E3467" t="n">
-        <v>51.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3467" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3468">
@@ -100709,10 +100709,10 @@
         <v>10350</v>
       </c>
       <c r="E3470" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3470" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3471">
@@ -100729,10 +100729,10 @@
         <v>10353</v>
       </c>
       <c r="E3471" t="n">
-        <v>42.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3471" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3472">
@@ -100749,10 +100749,10 @@
         <v>10356</v>
       </c>
       <c r="E3472" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3472" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3473">
@@ -100869,10 +100869,10 @@
         <v>10374</v>
       </c>
       <c r="E3478" t="n">
-        <v>104.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3478" t="n">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3479">
@@ -100889,10 +100889,10 @@
         <v>10377</v>
       </c>
       <c r="E3479" t="n">
-        <v>42.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3479" t="n">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3480">
@@ -100909,10 +100909,10 @@
         <v>10168</v>
       </c>
       <c r="E3480" t="n">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3480" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3481">

</xml_diff>